<commit_message>
obsługa trybu z timerem
</commit_message>
<xml_diff>
--- a/testy.xlsx
+++ b/testy.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="20730" windowHeight="11760"/>
@@ -153,8 +153,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,7 +191,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -204,9 +204,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -244,7 +244,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -278,6 +278,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -312,9 +313,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -487,21 +489,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="91.140625" customWidth="1"/>
     <col min="3" max="3" width="97.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -515,7 +517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -529,7 +531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -543,7 +545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -557,7 +559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -571,7 +573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -585,7 +587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -599,7 +601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -613,7 +615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -627,7 +629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -641,7 +643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -655,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -663,7 +665,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -677,7 +679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -691,7 +693,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -705,7 +707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -719,7 +721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -733,7 +735,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -747,7 +749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -761,7 +763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -775,7 +777,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -789,7 +791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -803,7 +805,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -817,92 +819,92 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -916,24 +918,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>